<commit_message>
added sheet with number of instances that have soln = lowerbound
</commit_message>
<xml_diff>
--- a/PAPER/ALL.xlsx
+++ b/PAPER/ALL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OPT Tables" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="CPU Time OLD" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="CPU Time NEW" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Comparison" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="number opt solns" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="32">
   <si>
     <t xml:space="preserve">N = 100</t>
   </si>
@@ -115,6 +116,12 @@
   <si>
     <t xml:space="preserve">opt sd</t>
   </si>
+  <si>
+    <t xml:space="preserve">number of instances where the number of strips in the solution = lower bound (out of 1000 instances)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentages</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +131,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -155,6 +162,21 @@
     </font>
     <font>
       <sz val="10.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -220,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,6 +292,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,14 +394,14 @@
   </sheetPr>
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z57" activeCellId="0" sqref="Z57"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3091,18 +3133,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="15" min="11" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="15" min="11" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5899,7 +5941,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.55"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7468,7 +7510,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L40" activeCellId="0" sqref="L40"/>
@@ -7476,22 +7518,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.55"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="11.3418367346939"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="0"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
       <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -7902,6 +7980,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
       <c r="B16" s="2" t="n">
         <f aca="false">AVERAGE(B5:B15 )</f>
         <v>0.192057636363636</v>
@@ -7914,6 +7993,7 @@
         <f aca="false">AVERAGE(D5:D15)</f>
         <v>0.796502727272727</v>
       </c>
+      <c r="E16" s="0"/>
       <c r="F16" s="2" t="n">
         <f aca="false">AVERAGE(F5:F15 )</f>
         <v>0.201862363636364</v>
@@ -7926,6 +8006,7 @@
         <f aca="false">AVERAGE(H5:H15)</f>
         <v>0.565025181818182</v>
       </c>
+      <c r="I16" s="0"/>
       <c r="J16" s="2" t="n">
         <f aca="false">AVERAGE(J5:J15)</f>
         <v>0.203205363636364</v>
@@ -7939,19 +8020,83 @@
         <v>0.228667454545454</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+    </row>
     <row r="20" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B20" s="0"/>
       <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
       <c r="G20" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
       <c r="K20" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -8362,6 +8507,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
       <c r="B34" s="2" t="n">
         <f aca="false">AVERAGE(B23:B33)</f>
         <v>5.71101090909091</v>
@@ -8374,6 +8520,7 @@
         <f aca="false">AVERAGE(D23:D33)</f>
         <v>14.0823127272727</v>
       </c>
+      <c r="E34" s="0"/>
       <c r="F34" s="2" t="n">
         <f aca="false">AVERAGE(F23:F33)</f>
         <v>5.71609545454545</v>
@@ -8386,6 +8533,7 @@
         <f aca="false">AVERAGE(H23:H33)</f>
         <v>10.5049981818182</v>
       </c>
+      <c r="I34" s="0"/>
       <c r="J34" s="2" t="n">
         <f aca="false">AVERAGE(J23:J33)</f>
         <v>5.59720090909091</v>
@@ -8399,19 +8547,83 @@
         <v>6.33802909090909</v>
       </c>
     </row>
+    <row r="35" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+      <c r="J36" s="0"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+      <c r="I37" s="0"/>
+      <c r="J37" s="0"/>
+      <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
+    </row>
     <row r="38" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B38" s="0"/>
       <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
       <c r="G38" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="J38" s="0"/>
       <c r="K38" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
@@ -8875,17 +9087,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N33" activeCellId="0" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="11.3418367346939"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>0</v>
@@ -8893,12 +9117,30 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
       <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -8924,6 +9166,7 @@
       <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="L4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -9311,6 +9554,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
       <c r="B16" s="2" t="n">
         <f aca="false">AVERAGE(B5:B15)</f>
         <v>10.2693372727273</v>
@@ -9319,6 +9563,7 @@
         <f aca="false">AVERAGE(C5:C15)</f>
         <v>0.796502727272727</v>
       </c>
+      <c r="D16" s="0"/>
       <c r="F16" s="2" t="n">
         <f aca="false">AVERAGE(F5:F15)</f>
         <v>8.88620727272727</v>
@@ -9327,6 +9572,7 @@
         <f aca="false">AVERAGE(G5:G15)</f>
         <v>0.565025181818182</v>
       </c>
+      <c r="H16" s="0"/>
       <c r="J16" s="2" t="n">
         <f aca="false">AVERAGE(J5:J15)</f>
         <v>5.09304545454545</v>
@@ -9335,11 +9581,69 @@
         <f aca="false">AVERAGE(K5:K15)</f>
         <v>0.228667454545454</v>
       </c>
+      <c r="L16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -9365,6 +9669,7 @@
       <c r="K22" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -9752,6 +10057,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
       <c r="B34" s="2" t="n">
         <f aca="false">AVERAGE(B23:B33)</f>
         <v>214.044790909091</v>
@@ -9760,6 +10066,7 @@
         <f aca="false">AVERAGE(C23:C33)</f>
         <v>14.0823127272727</v>
       </c>
+      <c r="D34" s="0"/>
       <c r="F34" s="2" t="n">
         <f aca="false">AVERAGE(F23:F33)</f>
         <v>190.365790909091</v>
@@ -9768,6 +10075,7 @@
         <f aca="false">AVERAGE(G23:G33)</f>
         <v>10.5049981818182</v>
       </c>
+      <c r="H34" s="0"/>
       <c r="J34" s="2" t="n">
         <f aca="false">AVERAGE(J23:J33)</f>
         <v>214.787290909091</v>
@@ -9776,11 +10084,69 @@
         <f aca="false">AVERAGE(K23:K33)</f>
         <v>6.33802909090909</v>
       </c>
+      <c r="L34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="J36" s="0"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+      <c r="J37" s="0"/>
+      <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="J38" s="0"/>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
@@ -9806,6 +10172,7 @@
       <c r="K40" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="L40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -10216,6 +10583,2767 @@
       <c r="K52" s="2" t="n">
         <f aca="false">AVERAGE(K41:K51)</f>
         <v>29.7975181818182</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Z51"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O46" activeCellId="0" sqref="O46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="9.09183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="14" width="9.09183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="5.83163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="14" width="9.09183673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="6.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="14" width="9.09183673469388"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="13" customFormat="true" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" s="13" customFormat="true" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <f aca="false">B5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <f aca="false">C5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <f aca="false">D5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="n">
+        <f aca="false">F5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="2" t="n">
+        <f aca="false">G5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <f aca="false">H5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2" t="n">
+        <f aca="false">J5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2" t="n">
+        <f aca="false">K5 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <f aca="false">L5 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <f aca="false">B6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <f aca="false">C6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <f aca="false">D6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2" t="n">
+        <f aca="false">F6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="2" t="n">
+        <f aca="false">G6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <f aca="false">H6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2" t="n">
+        <f aca="false">J6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="2" t="n">
+        <f aca="false">K6 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <f aca="false">L6 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <f aca="false">B7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <f aca="false">C7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <f aca="false">D7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2" t="n">
+        <f aca="false">F7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="2" t="n">
+        <f aca="false">G7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="2" t="n">
+        <f aca="false">H7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2" t="n">
+        <f aca="false">J7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="2" t="n">
+        <f aca="false">K7 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <f aca="false">L7 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <f aca="false">B8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <f aca="false">C8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <f aca="false">D8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2" t="n">
+        <f aca="false">F8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="2" t="n">
+        <f aca="false">G8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <f aca="false">H8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2" t="n">
+        <f aca="false">J8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="2" t="n">
+        <f aca="false">K8 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="2" t="n">
+        <f aca="false">L8 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <f aca="false">B9 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <f aca="false">C9 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <f aca="false">D9 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2" t="n">
+        <f aca="false">F9 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="2" t="n">
+        <f aca="false">G9 / 10</f>
+        <v>0.3</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <f aca="false">H9 / 10</f>
+        <v>0.1</v>
+      </c>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2" t="n">
+        <f aca="false">J9 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="2" t="n">
+        <f aca="false">K9 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="2" t="n">
+        <f aca="false">L9 / 10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>450</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O10" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <f aca="false">B10 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <f aca="false">C10 / 10</f>
+        <v>45</v>
+      </c>
+      <c r="R10" s="2" t="n">
+        <f aca="false">D10 / 10</f>
+        <v>0.3</v>
+      </c>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2" t="n">
+        <f aca="false">F10 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="2" t="n">
+        <f aca="false">G10 / 10</f>
+        <v>8.8</v>
+      </c>
+      <c r="V10" s="2" t="n">
+        <f aca="false">H10 / 10</f>
+        <v>1.6</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2" t="n">
+        <f aca="false">J10 / 10</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y10" s="2" t="n">
+        <f aca="false">K10 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="2" t="n">
+        <f aca="false">L10 / 10</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>169</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>141</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="O11" s="15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <f aca="false">B11 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2" t="n">
+        <f aca="false">C11 / 10</f>
+        <v>80</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <f aca="false">D11 / 10</f>
+        <v>7.4</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2" t="n">
+        <f aca="false">F11 / 10</f>
+        <v>1</v>
+      </c>
+      <c r="U11" s="2" t="n">
+        <f aca="false">G11 / 10</f>
+        <v>16.9</v>
+      </c>
+      <c r="V11" s="2" t="n">
+        <f aca="false">H11 / 10</f>
+        <v>14.1</v>
+      </c>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2" t="n">
+        <f aca="false">J11 / 10</f>
+        <v>0.8</v>
+      </c>
+      <c r="Y11" s="2" t="n">
+        <f aca="false">K11 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2" t="n">
+        <f aca="false">L11 / 10</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>843</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>415</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>407</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="O12" s="15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <f aca="false">B12 / 10</f>
+        <v>2.9</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <f aca="false">C12 / 10</f>
+        <v>84.3</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <f aca="false">D12 / 10</f>
+        <v>41.5</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2" t="n">
+        <f aca="false">F12 / 10</f>
+        <v>10.5</v>
+      </c>
+      <c r="U12" s="2" t="n">
+        <f aca="false">G12 / 10</f>
+        <v>19.4</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <f aca="false">H12 / 10</f>
+        <v>40.7</v>
+      </c>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2" t="n">
+        <f aca="false">J12 / 10</f>
+        <v>4.1</v>
+      </c>
+      <c r="Y12" s="2" t="n">
+        <f aca="false">K12 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="2" t="n">
+        <f aca="false">L12 / 10</f>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>298</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>839</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>804</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>424</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>218</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>667</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="O13" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P13" s="2" t="n">
+        <f aca="false">B13 / 10</f>
+        <v>29.8</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <f aca="false">C13 / 10</f>
+        <v>83.9</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <f aca="false">D13 / 10</f>
+        <v>80.4</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2" t="n">
+        <f aca="false">F13 / 10</f>
+        <v>42.4</v>
+      </c>
+      <c r="U13" s="2" t="n">
+        <f aca="false">G13 / 10</f>
+        <v>21.8</v>
+      </c>
+      <c r="V13" s="2" t="n">
+        <f aca="false">H13 / 10</f>
+        <v>66.7</v>
+      </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2" t="n">
+        <f aca="false">J13 / 10</f>
+        <v>7.5</v>
+      </c>
+      <c r="Y13" s="2" t="n">
+        <f aca="false">K13 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2" t="n">
+        <f aca="false">L13 / 10</f>
+        <v>9.7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>768</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>847</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>927</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>701</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>246</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>768</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="O14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <f aca="false">B14 / 10</f>
+        <v>76.8</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <f aca="false">C14 / 10</f>
+        <v>84.7</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <f aca="false">D14 / 10</f>
+        <v>92.7</v>
+      </c>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2" t="n">
+        <f aca="false">F14 / 10</f>
+        <v>70.1</v>
+      </c>
+      <c r="U14" s="2" t="n">
+        <f aca="false">G14 / 10</f>
+        <v>24.6</v>
+      </c>
+      <c r="V14" s="2" t="n">
+        <f aca="false">H14 / 10</f>
+        <v>76.8</v>
+      </c>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2" t="n">
+        <f aca="false">J14 / 10</f>
+        <v>10.7</v>
+      </c>
+      <c r="Y14" s="2" t="n">
+        <f aca="false">K14 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2" t="n">
+        <f aca="false">L14 / 10</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>945</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>849</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>945</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>788</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>246</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>788</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="O15" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <f aca="false">B15 / 10</f>
+        <v>94.5</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <f aca="false">C15 / 10</f>
+        <v>84.9</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <f aca="false">D15 / 10</f>
+        <v>94.5</v>
+      </c>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2" t="n">
+        <f aca="false">F15 / 10</f>
+        <v>78.8</v>
+      </c>
+      <c r="U15" s="2" t="n">
+        <f aca="false">G15 / 10</f>
+        <v>24.6</v>
+      </c>
+      <c r="V15" s="2" t="n">
+        <f aca="false">H15 / 10</f>
+        <v>78.8</v>
+      </c>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2" t="n">
+        <f aca="false">J15 / 10</f>
+        <v>11.3</v>
+      </c>
+      <c r="Y15" s="2" t="n">
+        <f aca="false">K15 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="2" t="n">
+        <f aca="false">L15 / 10</f>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O19" s="13"/>
+    </row>
+    <row r="20" s="13" customFormat="true" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="U20" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O21" s="13"/>
+    </row>
+    <row r="22" s="13" customFormat="true" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="U22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="V22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <f aca="false">B23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2" t="n">
+        <f aca="false">C23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="2" t="n">
+        <f aca="false">D23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="0"/>
+      <c r="T23" s="2" t="n">
+        <f aca="false">F23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U23" s="2" t="n">
+        <f aca="false">G23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V23" s="2" t="n">
+        <f aca="false">H23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W23" s="0"/>
+      <c r="X23" s="2" t="n">
+        <f aca="false">J23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="2" t="n">
+        <f aca="false">K23 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="2" t="n">
+        <f aca="false">L23 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P24" s="2" t="n">
+        <f aca="false">B24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="2" t="n">
+        <f aca="false">C24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="2" t="n">
+        <f aca="false">D24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S24" s="0"/>
+      <c r="T24" s="2" t="n">
+        <f aca="false">F24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="2" t="n">
+        <f aca="false">G24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V24" s="2" t="n">
+        <f aca="false">H24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W24" s="0"/>
+      <c r="X24" s="2" t="n">
+        <f aca="false">J24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="2" t="n">
+        <f aca="false">K24 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="2" t="n">
+        <f aca="false">L24 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <f aca="false">B25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2" t="n">
+        <f aca="false">C25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <f aca="false">D25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S25" s="0"/>
+      <c r="T25" s="2" t="n">
+        <f aca="false">F25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U25" s="2" t="n">
+        <f aca="false">G25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <f aca="false">H25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W25" s="0"/>
+      <c r="X25" s="2" t="n">
+        <f aca="false">J25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="2" t="n">
+        <f aca="false">K25 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="2" t="n">
+        <f aca="false">L25 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="P26" s="2" t="n">
+        <f aca="false">B26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2" t="n">
+        <f aca="false">C26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="2" t="n">
+        <f aca="false">D26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="0"/>
+      <c r="T26" s="2" t="n">
+        <f aca="false">F26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="2" t="n">
+        <f aca="false">G26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V26" s="2" t="n">
+        <f aca="false">H26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W26" s="0"/>
+      <c r="X26" s="2" t="n">
+        <f aca="false">J26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="2" t="n">
+        <f aca="false">K26 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="2" t="n">
+        <f aca="false">L26 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" s="15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="P27" s="2" t="n">
+        <f aca="false">B27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2" t="n">
+        <f aca="false">C27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <f aca="false">D27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="0"/>
+      <c r="T27" s="2" t="n">
+        <f aca="false">F27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U27" s="2" t="n">
+        <f aca="false">G27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <f aca="false">H27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W27" s="0"/>
+      <c r="X27" s="2" t="n">
+        <f aca="false">J27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="2" t="n">
+        <f aca="false">K27 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="2" t="n">
+        <f aca="false">L27 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>127</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P28" s="2" t="n">
+        <f aca="false">B28 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <f aca="false">C28 / 10</f>
+        <v>12.7</v>
+      </c>
+      <c r="R28" s="2" t="n">
+        <f aca="false">D28 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S28" s="0"/>
+      <c r="T28" s="2" t="n">
+        <f aca="false">F28 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="2" t="n">
+        <f aca="false">G28 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V28" s="2" t="n">
+        <f aca="false">H28 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W28" s="0"/>
+      <c r="X28" s="2" t="n">
+        <f aca="false">J28 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="2" t="n">
+        <f aca="false">K28 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="2" t="n">
+        <f aca="false">L28 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>268</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="P29" s="2" t="n">
+        <f aca="false">B29 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="2" t="n">
+        <f aca="false">C29 / 10</f>
+        <v>26.8</v>
+      </c>
+      <c r="R29" s="2" t="n">
+        <f aca="false">D29 / 10</f>
+        <v>0.2</v>
+      </c>
+      <c r="S29" s="0"/>
+      <c r="T29" s="2" t="n">
+        <f aca="false">F29 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U29" s="2" t="n">
+        <f aca="false">G29 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V29" s="2" t="n">
+        <f aca="false">H29 / 10</f>
+        <v>0.4</v>
+      </c>
+      <c r="W29" s="0"/>
+      <c r="X29" s="2" t="n">
+        <f aca="false">J29 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="2" t="n">
+        <f aca="false">K29 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="2" t="n">
+        <f aca="false">L29 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>272</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>202</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="P30" s="2" t="n">
+        <f aca="false">B30 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="2" t="n">
+        <f aca="false">C30 / 10</f>
+        <v>27.2</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <f aca="false">D30 / 10</f>
+        <v>20.2</v>
+      </c>
+      <c r="S30" s="0"/>
+      <c r="T30" s="2" t="n">
+        <f aca="false">F30 / 10</f>
+        <v>0.4</v>
+      </c>
+      <c r="U30" s="2" t="n">
+        <f aca="false">G30 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="2" t="n">
+        <f aca="false">H30 / 10</f>
+        <v>9.3</v>
+      </c>
+      <c r="W30" s="0"/>
+      <c r="X30" s="2" t="n">
+        <f aca="false">J30 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="2" t="n">
+        <f aca="false">K30 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="2" t="n">
+        <f aca="false">L30 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>303</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>615</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>226</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="16"/>
+      <c r="O31" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P31" s="2" t="n">
+        <f aca="false">B31 / 10</f>
+        <v>5.7</v>
+      </c>
+      <c r="Q31" s="2" t="n">
+        <f aca="false">C31 / 10</f>
+        <v>30.3</v>
+      </c>
+      <c r="R31" s="2" t="n">
+        <f aca="false">D31 / 10</f>
+        <v>61.5</v>
+      </c>
+      <c r="S31" s="0"/>
+      <c r="T31" s="2" t="n">
+        <f aca="false">F31 / 10</f>
+        <v>7.4</v>
+      </c>
+      <c r="U31" s="2" t="n">
+        <f aca="false">G31 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="2" t="n">
+        <f aca="false">H31 / 10</f>
+        <v>22.6</v>
+      </c>
+      <c r="W31" s="0"/>
+      <c r="X31" s="2" t="n">
+        <f aca="false">J31 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="2" t="n">
+        <f aca="false">K31 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="2" t="n">
+        <f aca="false">L31 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>546</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>307</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>736</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>242</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>273</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="P32" s="2" t="n">
+        <f aca="false">B32 / 10</f>
+        <v>54.6</v>
+      </c>
+      <c r="Q32" s="2" t="n">
+        <f aca="false">C32 / 10</f>
+        <v>30.7</v>
+      </c>
+      <c r="R32" s="2" t="n">
+        <f aca="false">D32 / 10</f>
+        <v>73.6</v>
+      </c>
+      <c r="S32" s="0"/>
+      <c r="T32" s="2" t="n">
+        <f aca="false">F32 / 10</f>
+        <v>24.2</v>
+      </c>
+      <c r="U32" s="2" t="n">
+        <f aca="false">G32 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V32" s="2" t="n">
+        <f aca="false">H32 / 10</f>
+        <v>27.3</v>
+      </c>
+      <c r="W32" s="0"/>
+      <c r="X32" s="2" t="n">
+        <f aca="false">J32 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y32" s="2" t="n">
+        <f aca="false">K32 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z32" s="2" t="n">
+        <f aca="false">L32 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>756</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>322</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>756</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>277</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>277</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" s="2" t="n">
+        <f aca="false">B33 / 10</f>
+        <v>75.6</v>
+      </c>
+      <c r="Q33" s="2" t="n">
+        <f aca="false">C33 / 10</f>
+        <v>32.2</v>
+      </c>
+      <c r="R33" s="2" t="n">
+        <f aca="false">D33 / 10</f>
+        <v>75.6</v>
+      </c>
+      <c r="S33" s="0"/>
+      <c r="T33" s="2" t="n">
+        <f aca="false">F33 / 10</f>
+        <v>27.7</v>
+      </c>
+      <c r="U33" s="2" t="n">
+        <f aca="false">G33 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V33" s="2" t="n">
+        <f aca="false">H33 / 10</f>
+        <v>27.7</v>
+      </c>
+      <c r="W33" s="0"/>
+      <c r="X33" s="2" t="n">
+        <f aca="false">J33 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y33" s="2" t="n">
+        <f aca="false">K33 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z33" s="2" t="n">
+        <f aca="false">L33 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O34" s="13"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O35" s="13"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O36" s="13"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O37" s="13"/>
+    </row>
+    <row r="38" s="13" customFormat="true" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O38" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q38" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="U38" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y38" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O39" s="13"/>
+    </row>
+    <row r="40" s="13" customFormat="true" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="P40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="R40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="U40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="V40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z40" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <f aca="false">B41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="2" t="n">
+        <f aca="false">C41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <f aca="false">D41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2" t="n">
+        <f aca="false">F41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U41" s="2" t="n">
+        <f aca="false">G41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V41" s="2" t="n">
+        <f aca="false">H41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2" t="n">
+        <f aca="false">J41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="2" t="n">
+        <f aca="false">K41 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z41" s="2" t="n">
+        <f aca="false">L41 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" s="15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P42" s="2" t="n">
+        <f aca="false">B42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="2" t="n">
+        <f aca="false">C42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <f aca="false">D42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2" t="n">
+        <f aca="false">F42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U42" s="2" t="n">
+        <f aca="false">G42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V42" s="2" t="n">
+        <f aca="false">H42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2" t="n">
+        <f aca="false">J42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y42" s="2" t="n">
+        <f aca="false">K42 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z42" s="2" t="n">
+        <f aca="false">L42 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P43" s="2" t="n">
+        <f aca="false">B43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="2" t="n">
+        <f aca="false">C43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <f aca="false">D43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2" t="n">
+        <f aca="false">F43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U43" s="2" t="n">
+        <f aca="false">G43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V43" s="2" t="n">
+        <f aca="false">H43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2" t="n">
+        <f aca="false">J43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y43" s="2" t="n">
+        <f aca="false">K43 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z43" s="2" t="n">
+        <f aca="false">L43 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="P44" s="2" t="n">
+        <f aca="false">B44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="2" t="n">
+        <f aca="false">C44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R44" s="2" t="n">
+        <f aca="false">D44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2" t="n">
+        <f aca="false">F44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U44" s="2" t="n">
+        <f aca="false">G44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V44" s="2" t="n">
+        <f aca="false">H44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2" t="n">
+        <f aca="false">J44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y44" s="2" t="n">
+        <f aca="false">K44 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z44" s="2" t="n">
+        <f aca="false">L44 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" s="15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="P45" s="2" t="n">
+        <f aca="false">B45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <f aca="false">C45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R45" s="2" t="n">
+        <f aca="false">D45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2" t="n">
+        <f aca="false">F45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U45" s="2" t="n">
+        <f aca="false">G45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V45" s="2" t="n">
+        <f aca="false">H45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2" t="n">
+        <f aca="false">J45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y45" s="2" t="n">
+        <f aca="false">K45 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z45" s="2" t="n">
+        <f aca="false">L45 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P46" s="2" t="n">
+        <f aca="false">B46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="2" t="n">
+        <f aca="false">C46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <f aca="false">D46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2" t="n">
+        <f aca="false">F46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U46" s="2" t="n">
+        <f aca="false">G46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V46" s="2" t="n">
+        <f aca="false">H46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2" t="n">
+        <f aca="false">J46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y46" s="2" t="n">
+        <f aca="false">K46 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z46" s="2" t="n">
+        <f aca="false">L46 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" s="15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="P47" s="2" t="n">
+        <f aca="false">B47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="2" t="n">
+        <f aca="false">C47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R47" s="2" t="n">
+        <f aca="false">D47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2" t="n">
+        <f aca="false">F47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U47" s="2" t="n">
+        <f aca="false">G47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V47" s="2" t="n">
+        <f aca="false">H47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2" t="n">
+        <f aca="false">J47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y47" s="2" t="n">
+        <f aca="false">K47 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z47" s="2" t="n">
+        <f aca="false">L47 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="F48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" s="15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="P48" s="2" t="n">
+        <f aca="false">B48 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="2" t="n">
+        <f aca="false">C48 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R48" s="2" t="n">
+        <f aca="false">D48 / 10</f>
+        <v>15.2</v>
+      </c>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2" t="n">
+        <f aca="false">F48 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U48" s="2" t="n">
+        <f aca="false">G48 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V48" s="2" t="n">
+        <f aca="false">H48 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2" t="n">
+        <f aca="false">J48 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y48" s="2" t="n">
+        <f aca="false">K48 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z48" s="2" t="n">
+        <f aca="false">L48 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>451</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P49" s="2" t="n">
+        <f aca="false">B49 / 10</f>
+        <v>2.8</v>
+      </c>
+      <c r="Q49" s="2" t="n">
+        <f aca="false">C49 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R49" s="2" t="n">
+        <f aca="false">D49 / 10</f>
+        <v>45.1</v>
+      </c>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2" t="n">
+        <f aca="false">F49 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U49" s="2" t="n">
+        <f aca="false">G49 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V49" s="2" t="n">
+        <f aca="false">H49 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2" t="n">
+        <f aca="false">J49 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y49" s="2" t="n">
+        <f aca="false">K49 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z49" s="2" t="n">
+        <f aca="false">L49 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>358</v>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>527</v>
+      </c>
+      <c r="F50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="P50" s="2" t="n">
+        <f aca="false">B50 / 10</f>
+        <v>35.8</v>
+      </c>
+      <c r="Q50" s="2" t="n">
+        <f aca="false">C50 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R50" s="2" t="n">
+        <f aca="false">D50 / 10</f>
+        <v>52.7</v>
+      </c>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2" t="n">
+        <f aca="false">F50 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U50" s="2" t="n">
+        <f aca="false">G50 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V50" s="2" t="n">
+        <f aca="false">H50 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2" t="n">
+        <f aca="false">J50 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y50" s="2" t="n">
+        <f aca="false">K50 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z50" s="2" t="n">
+        <f aca="false">L50 / 10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>540</v>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>540</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P51" s="2" t="n">
+        <f aca="false">B51 / 10</f>
+        <v>54</v>
+      </c>
+      <c r="Q51" s="2" t="n">
+        <f aca="false">C51 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="R51" s="2" t="n">
+        <f aca="false">D51 / 10</f>
+        <v>54</v>
+      </c>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2" t="n">
+        <f aca="false">F51 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="U51" s="2" t="n">
+        <f aca="false">G51 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="V51" s="2" t="n">
+        <f aca="false">H51 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2" t="n">
+        <f aca="false">J51 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Y51" s="2" t="n">
+        <f aca="false">K51 / 10</f>
+        <v>0</v>
+      </c>
+      <c r="Z51" s="2" t="n">
+        <f aca="false">L51 / 10</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>